<commit_message>
[web] - firefox headless and chrome headless driver are also supported as part of the auto-driver-download feature - [`assertTextMatches(text,minMatch,scrollTo)`](../commands/web/assertTextMatches(text,minMatch,scrollTo)) - assert the   minimum number of occurrence of `text` in current web page, and optionally scroll to the specified instance. - fixed error when automating scrolling on an element that might not support scrolling (e.g. Window, Document, Html)
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-02.data.xlsx
+++ b/artifact/data/web-02.data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D6256B-29BE-324C-B94A-BA0B54353093}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4685273B-83F7-D545-9658-988FFD6569AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="440" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="7840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
-    <sheet name="#default (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="test" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -37,7 +37,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -50,42 +50,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>nexial.scope.fallbackToPrevious</t>
+  </si>
+  <si>
+    <t>nexial.pollWaitMs</t>
+  </si>
+  <si>
+    <t>nexial.failFast</t>
+  </si>
+  <si>
+    <t>nexial.textDelim</t>
+  </si>
+  <si>
+    <t>nexial.verbose</t>
+  </si>
+  <si>
+    <t>nexial.openResult</t>
+  </si>
+  <si>
+    <t>750</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>nexial.scope.iteration</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>nexial.scope.fallbackToPrevious</t>
-  </si>
-  <si>
-    <t>nexial.scope.iteration</t>
-  </si>
-  <si>
-    <t>nexial.pollWaitMs</t>
-  </si>
-  <si>
-    <t>nexial.failFast</t>
-  </si>
-  <si>
-    <t>nexial.textDelim</t>
-  </si>
-  <si>
-    <t>nexial.verbose</t>
-  </si>
-  <si>
-    <t>nexial.openResult</t>
+    <t>//nexial.highlightWaitMs</t>
+  </si>
+  <si>
+    <t>//nexial.highlight</t>
   </si>
 </sst>
 </file>
@@ -214,72 +223,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -701,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA9"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -716,7 +660,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -726,47 +670,47 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -775,10 +719,22 @@
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
@@ -789,21 +745,21 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -813,11 +769,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41FD73F-F46B-8846-B902-2CCE56A22837}">
-  <dimension ref="A1:AAA10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02992098-561F-1944-A340-34CB95735B3B}">
+  <dimension ref="A1:AAA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -831,10 +787,10 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
@@ -844,8 +800,8 @@
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="HA4" s="4"/>
@@ -871,32 +827,9 @@
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
-    <row r="10" spans="1:703">
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
-      <formula>LEN(TRIM(B2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
@@ -907,7 +840,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1">
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>

</xml_diff>

<commit_message>
- fixed missing byte array to string conversion in `web >> savePageAs(var,sessionIdName,url)`
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-02.data.xlsx
+++ b/artifact/data/web-02.data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4685273B-83F7-D545-9658-988FFD6569AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A549DA-ABA3-C943-B0DB-7073EA067CCF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="7840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="7840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
-    <sheet name="test" sheetId="3" r:id="rId2"/>
+    <sheet name="browser" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>true</t>
   </si>
@@ -95,6 +95,42 @@
   </si>
   <si>
     <t>//nexial.highlight</t>
+  </si>
+  <si>
+    <t>aut : url</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/%22Hello,_World!%22_program</t>
+  </si>
+  <si>
+    <t>aut : links</t>
+  </si>
+  <si>
+    <t>computer program,programming languages,syntax,Bell Laboratories,Go programming language,good enough,GNU Hello,Java Pet Store</t>
+  </si>
+  <si>
+    <t>aut : unexpected</t>
+  </si>
+  <si>
+    <t>Nexial Automation</t>
+  </si>
+  <si>
+    <t>aut : expected</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>1997 Lucent Technologies Inc. All rights reserved.</t>
+  </si>
+  <si>
+    <t>"The Programming Language B"</t>
+  </si>
+  <si>
+    <t>aut : link label to B</t>
+  </si>
+  <si>
+    <t>B : copyright</t>
   </si>
 </sst>
 </file>
@@ -645,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -713,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
@@ -772,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02992098-561F-1944-A340-34CB95735B3B}">
   <dimension ref="A1:AAA9"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -796,26 +832,62 @@
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>

</xml_diff>